<commit_message>
Data item columns providers + tests
</commit_message>
<xml_diff>
--- a/ExcelReporter.Tests/TestData/DataSourcePanelDictionaryRenderTest/TestRenderDictionary.xlsx
+++ b/ExcelReporter.Tests/TestData/DataSourcePanelDictionaryRenderTest/TestRenderDictionary.xlsx
@@ -14,15 +14,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <x:si>
+    <x:t>Key</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Value</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Name</x:t>
+  </x:si>
   <x:si>
     <x:t>Name_1</x:t>
   </x:si>
   <x:si>
-    <x:t>Name_2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Name_3</x:t>
+    <x:t>IsVip</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -373,42 +379,65 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:D4"/>
+  <x:dimension ref="A1:F6"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="2" spans="1:4">
+    <x:row r="1" spans="1:6">
+      <x:c r="B1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E1" s="0" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:6">
       <x:c r="B2" s="0" t="s">
-        <x:v>0</x:v>
-      </x:c>
-      <x:c r="C2" s="0" t="n">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:6">
+      <x:c r="B3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="n">
         <x:v>25.7</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="b">
-        <x:v>1</x:v>
+      <x:c r="E3" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="n">
+        <x:v>25.7</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:4">
-      <x:c r="B3" s="0" t="s">
-        <x:v>1</x:v>
-      </x:c>
-      <x:c r="C3" s="0" t="n">
-        <x:v>250.7</x:v>
-      </x:c>
-      <x:c r="D3" s="0" t="b">
-        <x:v>0</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:4">
+    <x:row r="4" spans="1:6">
       <x:c r="B4" s="0" t="s">
-        <x:v>2</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="n">
-        <x:v>2500.7</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="b">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="b">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
     </x:row>

</xml_diff>